<commit_message>
TICKET2383 - Consolidated Report - Updated Excel Spreadsheet
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3617 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-2.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-2.xlsx
@@ -12,17 +12,15 @@
     <sheet name="Activity Summary" sheetId="9" r:id="rId3"/>
     <sheet name="Bookings" sheetId="10" r:id="rId4"/>
     <sheet name="Impressions" sheetId="7" r:id="rId5"/>
-    <sheet name="Leads By Geo" sheetId="12" r:id="rId6"/>
-    <sheet name="Contact Details" sheetId="8" r:id="rId7"/>
-    <sheet name="Key - Legend" sheetId="6" r:id="rId8"/>
+    <sheet name="Contact Details" sheetId="8" r:id="rId6"/>
+    <sheet name="Key - Legend" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Activity Summary'!$A$1:$I$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Bookings!$A$1:$I$27</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Contact Details'!$A$1:$S$93</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Contact Details'!$A$1:$S$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Impressions!$A$1:$P$29</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Leads By Geo'!$A$1:$I$62</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'Contact Details'!$9:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Contact Details'!$9:$9</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -68,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="130">
   <si>
     <t>calls</t>
   </si>
@@ -271,9 +269,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>Call Duration</t>
   </si>
   <si>
@@ -332,153 +327,6 @@
   </si>
   <si>
     <t>Value to Date</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>(not set)</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Iowa</t>
   </si>
   <si>
     <t>ROI (YTD):</t>
@@ -542,18 +390,6 @@
   </si>
   <si>
     <t>Anonymous view of your dedicated promotional page on an LLTG site, or a view of your listing, description, photo, video, or advertisment by an A.T.</t>
-  </si>
-  <si>
-    <t>Non-US</t>
-  </si>
-  <si>
-    <t>Other States</t>
-  </si>
-  <si>
-    <t>Affluent Traveler Activity, By State</t>
-  </si>
-  <si>
-    <t>includes Emails, Leads, Calls and Bookings</t>
   </si>
   <si>
     <t>Email Address / Email</t>
@@ -640,7 +476,7 @@
     <numFmt numFmtId="170" formatCode="0.0%"/>
     <numFmt numFmtId="171" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -764,12 +600,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -792,13 +622,6 @@
       <b/>
       <sz val="18"/>
       <color rgb="FF008ACD"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1064,7 +887,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1282,9 +1105,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1323,7 +1143,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1331,16 +1151,14 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="24" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="24" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="23" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="24" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="23" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1355,14 +1173,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="9" fontId="22" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="21" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="6" fontId="22" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="21" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1370,16 +1188,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="22" fillId="5" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="5" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="25" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="26" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1517,6 +1332,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -2352,11 +2168,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="85764736"/>
-        <c:axId val="85774720"/>
+        <c:axId val="45847680"/>
+        <c:axId val="45849216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85764736"/>
+        <c:axId val="45847680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85774720"/>
+        <c:crossAx val="45849216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2392,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85774720"/>
+        <c:axId val="45849216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2236,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85764736"/>
+        <c:crossAx val="45847680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2636,143 +2452,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Leads By Geo'!$A$9:$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>Non-US</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Other States</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>California</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>New York</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Texas</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Illinois</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Pennsylvania</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>New Jersey</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Florida</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Georgia</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Massachusetts</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Connecticut</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>District of Columbia</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Kentucky</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Virginia</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Ohio</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Arizona</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>North Carolina</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Washington</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Colorado</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>South Carolina</c:v>
-                </c:pt>
-              </c:strCache>
+              <c:f>#REF!</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leads By Geo'!$B$9:$B$29</c:f>
+              <c:f>#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>19</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2788,12 +2478,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="88036480"/>
-        <c:axId val="88038016"/>
+        <c:axId val="45866368"/>
+        <c:axId val="45626496"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88036480"/>
+        <c:axId val="45866368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,7 +2501,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88038016"/>
+        <c:crossAx val="45626496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2819,7 +2509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88038016"/>
+        <c:axId val="45626496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2847,7 +2537,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88036480"/>
+        <c:crossAx val="45866368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2924,6 +2614,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3111,12 +2802,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="88079744"/>
-        <c:axId val="89265280"/>
+        <c:axId val="45655936"/>
+        <c:axId val="45657472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88079744"/>
+        <c:axId val="45655936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,7 +2835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89265280"/>
+        <c:crossAx val="45657472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3152,7 +2843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89265280"/>
+        <c:axId val="45657472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3180,7 +2871,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88079744"/>
+        <c:crossAx val="45655936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3424,12 +3115,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="89299584"/>
-        <c:axId val="89301376"/>
+        <c:axId val="45696128"/>
+        <c:axId val="45697664"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="89299584"/>
+        <c:axId val="45696128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3457,7 +3148,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89301376"/>
+        <c:crossAx val="45697664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3465,7 +3156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89301376"/>
+        <c:axId val="45697664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3493,7 +3184,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89299584"/>
+        <c:crossAx val="45696128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3570,6 +3261,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3686,11 +3378,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="89920256"/>
-        <c:axId val="89921792"/>
+        <c:axId val="45710336"/>
+        <c:axId val="45740800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89920256"/>
+        <c:axId val="45710336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3718,7 +3410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89921792"/>
+        <c:crossAx val="45740800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3726,7 +3418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89921792"/>
+        <c:axId val="45740800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,7 +3428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89920256"/>
+        <c:crossAx val="45710336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4134,16 +3826,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4167,7 +3859,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5095875" y="0"/>
+          <a:off x="4467225" y="9525"/>
           <a:ext cx="2114550" cy="704850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4280,79 +3972,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="285737" name="Picture 1" descr="LLTG_logo 190x50.gif"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4933950" y="0"/>
-          <a:ext cx="2114550" cy="676275"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -4422,7 +4041,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5468,7 +5087,7 @@
   <dimension ref="A1:P115"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5498,7 +5117,7 @@
       <c r="H1" s="49"/>
       <c r="I1" s="42"/>
       <c r="J1" s="48" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="K1" s="42"/>
       <c r="L1" s="42"/>
@@ -5534,13 +5153,13 @@
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="H3" s="49"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="149"/>
-      <c r="M3" s="149"/>
-      <c r="N3" s="149"/>
-      <c r="O3" s="150"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="145"/>
       <c r="P3" s="42"/>
     </row>
     <row r="4" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
@@ -5552,13 +5171,13 @@
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
       <c r="H4" s="49"/>
-      <c r="I4" s="151"/>
-      <c r="J4" s="159"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="49"/>
-      <c r="O4" s="152"/>
+      <c r="O4" s="147"/>
       <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
@@ -5570,32 +5189,32 @@
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
       <c r="H5" s="49"/>
-      <c r="I5" s="151"/>
-      <c r="J5" s="146"/>
-      <c r="K5" s="127"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="124"/>
       <c r="L5" s="47"/>
       <c r="M5" s="49"/>
       <c r="N5" s="49"/>
-      <c r="O5" s="152"/>
+      <c r="O5" s="147"/>
       <c r="P5" s="42"/>
     </row>
-    <row r="6" spans="1:16" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="129"/>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="130"/>
-      <c r="K6" s="130"/>
-      <c r="L6" s="130"/>
-      <c r="M6" s="130"/>
+    <row r="6" spans="1:16" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
       <c r="N6" s="49"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="129"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="126"/>
     </row>
     <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
@@ -5606,15 +5225,15 @@
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
       <c r="H7" s="49"/>
-      <c r="I7" s="151"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="128" t="s">
-        <v>147</v>
+      <c r="I7" s="146"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="125" t="s">
+        <v>97</v>
       </c>
       <c r="L7" s="49"/>
       <c r="M7" s="49"/>
       <c r="N7" s="49"/>
-      <c r="O7" s="152"/>
+      <c r="O7" s="147"/>
       <c r="P7" s="42"/>
     </row>
     <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5626,18 +5245,18 @@
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
       <c r="H8" s="49"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="147" t="e">
+      <c r="I8" s="146"/>
+      <c r="J8" s="142" t="e">
         <f>'Activity Summary'!I31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="128" t="s">
-        <v>163</v>
+      <c r="K8" s="125" t="s">
+        <v>109</v>
       </c>
       <c r="L8" s="49"/>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
-      <c r="O8" s="152"/>
+      <c r="O8" s="147"/>
       <c r="P8" s="42"/>
     </row>
     <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5649,18 +5268,18 @@
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="H9" s="49"/>
-      <c r="I9" s="151"/>
-      <c r="J9" s="147">
+      <c r="I9" s="146"/>
+      <c r="J9" s="142">
         <f>Bookings!E22</f>
         <v>0</v>
       </c>
-      <c r="K9" s="128" t="s">
-        <v>169</v>
+      <c r="K9" s="125" t="s">
+        <v>115</v>
       </c>
       <c r="L9" s="49"/>
       <c r="M9" s="49"/>
       <c r="N9" s="49"/>
-      <c r="O9" s="152"/>
+      <c r="O9" s="147"/>
       <c r="P9" s="42"/>
     </row>
     <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5672,18 +5291,18 @@
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
       <c r="H10" s="49"/>
-      <c r="I10" s="151"/>
-      <c r="J10" s="147" t="e">
+      <c r="I10" s="146"/>
+      <c r="J10" s="142" t="e">
         <f>J8+J9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="128" t="s">
-        <v>175</v>
+      <c r="K10" s="125" t="s">
+        <v>121</v>
       </c>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
       <c r="N10" s="49"/>
-      <c r="O10" s="152"/>
+      <c r="O10" s="147"/>
       <c r="P10" s="42"/>
     </row>
     <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5695,18 +5314,18 @@
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="49"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="144" t="e">
+      <c r="I11" s="146"/>
+      <c r="J11" s="139" t="e">
         <f>J10/J7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="128" t="s">
-        <v>137</v>
+      <c r="K11" s="125" t="s">
+        <v>87</v>
       </c>
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
-      <c r="O11" s="152"/>
+      <c r="O11" s="147"/>
       <c r="P11" s="42"/>
     </row>
     <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.25">
@@ -5718,13 +5337,13 @@
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="H12" s="49"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="155"/>
-      <c r="K12" s="156"/>
-      <c r="L12" s="157"/>
-      <c r="M12" s="157"/>
-      <c r="N12" s="157"/>
-      <c r="O12" s="158"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="151"/>
+      <c r="L12" s="152"/>
+      <c r="M12" s="152"/>
+      <c r="N12" s="152"/>
+      <c r="O12" s="153"/>
       <c r="P12" s="42"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -7555,8 +7174,8 @@
       <c r="J114" s="42"/>
       <c r="K114" s="42"/>
       <c r="L114" s="42"/>
-      <c r="O114" s="142" t="s">
-        <v>182</v>
+      <c r="O114" s="137" t="s">
+        <v>128</v>
       </c>
       <c r="P114" s="42"/>
     </row>
@@ -7599,8 +7218,8 @@
   </sheetPr>
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7618,7 +7237,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -7641,7 +7260,7 @@
       <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="136">
+      <c r="A3" s="131">
         <f>Dashboard!$J$4</f>
         <v>0</v>
       </c>
@@ -7655,11 +7274,11 @@
       <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="161" t="s">
-        <v>142</v>
+      <c r="A4" s="155" t="s">
+        <v>92</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="53"/>
@@ -7670,12 +7289,12 @@
       <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="162">
+      <c r="A5" s="156">
         <f>Dashboard!J7</f>
         <v>0</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="53"/>
@@ -7686,11 +7305,11 @@
       <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="161" t="s">
-        <v>173</v>
+      <c r="A6" s="155" t="s">
+        <v>119</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="53"/>
@@ -7701,8 +7320,8 @@
       <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="163" t="s">
-        <v>174</v>
+      <c r="A7" s="157" t="s">
+        <v>120</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="54"/>
@@ -7726,7 +7345,7 @@
     </row>
     <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -7758,7 +7377,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>32</v>
@@ -7788,7 +7407,7 @@
         <f>Impressions!F10</f>
         <v>0</v>
       </c>
-      <c r="G11" s="164" t="e">
+      <c r="G11" s="158" t="e">
         <f>G26/5</f>
         <v>#DIV/0!</v>
       </c>
@@ -7806,7 +7425,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="8">
         <f>0.03*B11</f>
@@ -7845,7 +7464,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="B13" s="8">
         <v>99</v>
@@ -7883,7 +7502,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="8">
         <v>125</v>
@@ -7959,7 +7578,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="23" t="e">
@@ -7997,7 +7616,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="8">
         <f>Bookings!C7</f>
@@ -8037,7 +7656,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="28" t="e">
@@ -8135,7 +7754,7 @@
         <v>32</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I25" s="37" t="s">
         <v>32</v>
@@ -8184,7 +7803,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="8">
         <f>B12*5</f>
@@ -8224,7 +7843,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="B28" s="8">
         <f>B13*5</f>
@@ -8265,7 +7884,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="8">
         <f>B14*5</f>
@@ -8350,7 +7969,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="23" t="e">
@@ -8391,7 +8010,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="8">
         <f>Bookings!C18</f>
@@ -8435,7 +8054,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="28" t="e">
@@ -8522,7 +8141,7 @@
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="143" t="str">
+      <c r="G40" s="138" t="str">
         <f>Dashboard!$O$114</f>
         <v>Please see Key for Descriptions</v>
       </c>
@@ -8998,17 +8617,16 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F28" sqref="F28:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
@@ -9018,7 +8636,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -9030,7 +8648,7 @@
       <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="137">
+      <c r="A2" s="132">
         <f>Dashboard!$J$4</f>
         <v>0</v>
       </c>
@@ -9044,10 +8662,10 @@
       <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="139"/>
+      <c r="A3" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="134"/>
       <c r="C3" s="55"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -9057,7 +8675,7 @@
       <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
       <c r="D4" s="42"/>
@@ -9079,24 +8697,27 @@
       <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="134" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="134" t="s">
+      <c r="A6" s="34">
+        <f>'Activity Summary'!A10</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="129" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="134" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" s="134" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="134" t="s">
-        <v>166</v>
+      <c r="E6" s="129" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="129" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -9141,7 +8762,7 @@
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="165"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="17">
@@ -9195,14 +8816,14 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="14"/>
       <c r="F12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="14"/>
       <c r="F13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="28">
         <f>G11-G12</f>
@@ -9237,26 +8858,27 @@
       <c r="G16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="134" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="134" t="s">
+      <c r="A17" s="34">
+        <f>'Activity Summary'!A25</f>
+        <v>0</v>
+      </c>
+      <c r="B17" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="129" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="134" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" s="134" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="134" t="s">
-        <v>166</v>
+      <c r="E17" s="129" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="129" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -9355,13 +8977,13 @@
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F24" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G24" s="28">
         <f>G22-G23</f>
@@ -9384,7 +9006,7 @@
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
-      <c r="F26" s="123"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
@@ -9406,12 +9028,12 @@
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="166" t="s">
-        <v>167</v>
-      </c>
-      <c r="I28" s="166"/>
+      <c r="F28" s="160" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
@@ -9419,10 +9041,10 @@
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>
       <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="166"/>
-      <c r="I29" s="166"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="42"/>
@@ -9441,12 +9063,11 @@
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="143" t="str">
+      <c r="F31" s="138" t="str">
         <f>Dashboard!$O$114</f>
         <v>Please see Key for Descriptions</v>
       </c>
+      <c r="G31" s="42"/>
       <c r="I31" s="42"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -9604,12 +9225,13 @@
       <c r="I45" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H28:I29"/>
+    <mergeCell ref="F28:G29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H31" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
+    <hyperlink ref="F31" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="99" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9643,7 +9265,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -9662,7 +9284,7 @@
       <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="135">
+      <c r="A2" s="130">
         <f>Dashboard!$J$4</f>
         <v>0</v>
       </c>
@@ -9684,7 +9306,7 @@
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="106" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="B3" s="107"/>
       <c r="C3" s="108"/>
@@ -9703,9 +9325,9 @@
       <c r="P3" s="42"/>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="112"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
       <c r="D4" s="64"/>
       <c r="E4" s="64"/>
       <c r="F4" s="64"/>
@@ -9721,9 +9343,9 @@
       <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
+      <c r="A5" s="109"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
       <c r="D5" s="64"/>
       <c r="E5" s="64"/>
       <c r="F5" s="64"/>
@@ -9772,11 +9394,11 @@
       <c r="K7" s="33"/>
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
-      <c r="N7" s="120" t="s">
+      <c r="N7" s="117" t="s">
         <v>46</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P7" s="42"/>
     </row>
@@ -10078,19 +9700,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="120" t="s">
+      <c r="N18" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="O18" s="121" t="s">
-        <v>87</v>
+      <c r="O18" s="118" t="s">
+        <v>86</v>
       </c>
       <c r="P18" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -10118,7 +9740,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -10146,7 +9768,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -10174,7 +9796,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -10202,7 +9824,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -10230,7 +9852,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -10258,7 +9880,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -10483,7 +10105,7 @@
       <c r="K34" s="42"/>
       <c r="L34" s="42"/>
       <c r="M34" s="42"/>
-      <c r="N34" s="143" t="str">
+      <c r="N34" s="138" t="str">
         <f>Dashboard!$O$114</f>
         <v>Please see Key for Descriptions</v>
       </c>
@@ -10991,973 +10613,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I65"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" style="109" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.85546875" style="109"/>
-    <col min="9" max="9" width="15.85546875" style="109" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="109"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="104" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="131" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="131"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-    </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="137">
-        <f>Dashboard!$J$4</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="160"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="111"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="111"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="133" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="133" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="132" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="132">
-        <v>32</v>
-      </c>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="110" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="110">
-        <v>178</v>
-      </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="110" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="110">
-        <v>222</v>
-      </c>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="110" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="110">
-        <v>167</v>
-      </c>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="110" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="110">
-        <v>121</v>
-      </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="110">
-        <v>89</v>
-      </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="111"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="110">
-        <v>73</v>
-      </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="110" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="110">
-        <v>66</v>
-      </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="110" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="110">
-        <v>53</v>
-      </c>
-      <c r="C17" s="111"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="110" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="110">
-        <v>44</v>
-      </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="110" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="110">
-        <v>40</v>
-      </c>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="110" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="110">
-        <v>35</v>
-      </c>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="110" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="110">
-        <v>33</v>
-      </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="110" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="110">
-        <v>32</v>
-      </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="111"/>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="110" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="110">
-        <v>30</v>
-      </c>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="110" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="110">
-        <v>29</v>
-      </c>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="110" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="110">
-        <v>27</v>
-      </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="110" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="110">
-        <v>26</v>
-      </c>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="110" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="110">
-        <v>25</v>
-      </c>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="110" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="110">
-        <v>20</v>
-      </c>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="B29" s="110">
-        <v>19</v>
-      </c>
-      <c r="C29" s="111"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="111"/>
-      <c r="I29" s="111"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C30" s="111"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
-      <c r="I30" s="111"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="110" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="110">
-        <v>10</v>
-      </c>
-      <c r="C31" s="111"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="111"/>
-      <c r="H31" s="111"/>
-      <c r="I31" s="111"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="110" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="110">
-        <v>9</v>
-      </c>
-      <c r="C32" s="111"/>
-      <c r="D32" s="111"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="111"/>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="110" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="110">
-        <v>9</v>
-      </c>
-      <c r="C33" s="111"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="111"/>
-      <c r="I33" s="111"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="110" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="110">
-        <v>9</v>
-      </c>
-      <c r="C34" s="111"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="110" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="110">
-        <v>8</v>
-      </c>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="110" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="110">
-        <v>7</v>
-      </c>
-      <c r="C36" s="111"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="111"/>
-      <c r="F36" s="111"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="110">
-        <v>7</v>
-      </c>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="110" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="110">
-        <v>6</v>
-      </c>
-      <c r="C38" s="111"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="110" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="110">
-        <v>6</v>
-      </c>
-      <c r="C39" s="111"/>
-      <c r="D39" s="111"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="111"/>
-      <c r="H39" s="111"/>
-      <c r="I39" s="111"/>
-    </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="110" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="110">
-        <v>5</v>
-      </c>
-      <c r="C40" s="111"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="110" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="110">
-        <v>4</v>
-      </c>
-      <c r="C41" s="111"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="111"/>
-      <c r="I41" s="111"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="110" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="110">
-        <v>4</v>
-      </c>
-      <c r="C42" s="111"/>
-      <c r="D42" s="111"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="111"/>
-      <c r="G42" s="111"/>
-      <c r="H42" s="111"/>
-      <c r="I42" s="111"/>
-    </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="110" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="110">
-        <v>4</v>
-      </c>
-      <c r="C43" s="111"/>
-      <c r="D43" s="111"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="111"/>
-      <c r="G43" s="111"/>
-      <c r="H43" s="111"/>
-      <c r="I43" s="111"/>
-    </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="110" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="110">
-        <v>3</v>
-      </c>
-      <c r="C44" s="111"/>
-      <c r="D44" s="111"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="111"/>
-      <c r="G44" s="111"/>
-      <c r="H44" s="111"/>
-      <c r="I44" s="111"/>
-    </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="110" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="110">
-        <v>3</v>
-      </c>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="110" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="110">
-        <v>3</v>
-      </c>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="110" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="110">
-        <v>2</v>
-      </c>
-      <c r="C47" s="111"/>
-      <c r="D47" s="111"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="111"/>
-      <c r="H47" s="111"/>
-      <c r="I47" s="111"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="110" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="110">
-        <v>2</v>
-      </c>
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="110" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="110">
-        <v>2</v>
-      </c>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="110" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="110">
-        <v>2</v>
-      </c>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-    </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="110" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="110">
-        <v>2</v>
-      </c>
-      <c r="C51" s="111"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-    </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="110" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="110">
-        <v>1</v>
-      </c>
-      <c r="C52" s="111"/>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="111"/>
-      <c r="I52" s="111"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="110">
-        <v>1</v>
-      </c>
-      <c r="C53" s="111"/>
-      <c r="D53" s="111"/>
-      <c r="E53" s="111"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="111"/>
-      <c r="I53" s="111"/>
-    </row>
-    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="110" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="110">
-        <v>1</v>
-      </c>
-      <c r="C54" s="111"/>
-      <c r="D54" s="111"/>
-      <c r="E54" s="111"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="111"/>
-      <c r="I54" s="111"/>
-    </row>
-    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="110" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="110">
-        <v>0</v>
-      </c>
-      <c r="C55" s="111"/>
-      <c r="D55" s="111"/>
-      <c r="E55" s="111"/>
-      <c r="F55" s="111"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="111"/>
-      <c r="I55" s="111"/>
-    </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="110" t="s">
-        <v>131</v>
-      </c>
-      <c r="B56" s="110">
-        <v>0</v>
-      </c>
-      <c r="C56" s="111"/>
-      <c r="D56" s="111"/>
-      <c r="E56" s="111"/>
-      <c r="F56" s="111"/>
-      <c r="G56" s="111"/>
-      <c r="H56" s="111"/>
-      <c r="I56" s="111"/>
-    </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="110" t="s">
-        <v>132</v>
-      </c>
-      <c r="B57" s="110">
-        <v>0</v>
-      </c>
-      <c r="C57" s="111"/>
-      <c r="D57" s="111"/>
-      <c r="E57" s="111"/>
-      <c r="F57" s="111"/>
-      <c r="G57" s="111"/>
-      <c r="H57" s="111"/>
-      <c r="I57" s="111"/>
-    </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="110" t="s">
-        <v>133</v>
-      </c>
-      <c r="B58" s="110">
-        <v>0</v>
-      </c>
-      <c r="C58" s="111"/>
-      <c r="D58" s="111"/>
-      <c r="E58" s="111"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-    </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="110" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="110">
-        <v>0</v>
-      </c>
-      <c r="C59" s="111"/>
-      <c r="D59" s="111"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="111"/>
-      <c r="I59" s="111"/>
-    </row>
-    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="110" t="s">
-        <v>135</v>
-      </c>
-      <c r="B60" s="110">
-        <v>0</v>
-      </c>
-      <c r="C60" s="111"/>
-      <c r="D60" s="111"/>
-      <c r="E60" s="111"/>
-      <c r="F60" s="111"/>
-      <c r="G60" s="143" t="str">
-        <f>Dashboard!$O$114</f>
-        <v>Please see Key for Descriptions</v>
-      </c>
-      <c r="H60" s="111"/>
-      <c r="I60" s="111"/>
-    </row>
-    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="110" t="s">
-        <v>136</v>
-      </c>
-      <c r="B61" s="110">
-        <v>0</v>
-      </c>
-      <c r="C61" s="111"/>
-      <c r="D61" s="111"/>
-      <c r="E61" s="111"/>
-      <c r="F61" s="111"/>
-      <c r="G61" s="111"/>
-      <c r="H61" s="111"/>
-      <c r="I61" s="111"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="111"/>
-      <c r="B62" s="111">
-        <f>SUM(B10:B61)</f>
-        <v>1439</v>
-      </c>
-      <c r="C62" s="111"/>
-      <c r="D62" s="111"/>
-      <c r="E62" s="111"/>
-      <c r="F62" s="111"/>
-      <c r="G62" s="111"/>
-      <c r="H62" s="111"/>
-      <c r="I62" s="111"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="111"/>
-      <c r="B63" s="111"/>
-      <c r="C63" s="111"/>
-      <c r="D63" s="111"/>
-      <c r="E63" s="111"/>
-      <c r="F63" s="111"/>
-      <c r="G63" s="111"/>
-      <c r="H63" s="111"/>
-      <c r="I63" s="111"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="111"/>
-      <c r="B64" s="111"/>
-      <c r="C64" s="111"/>
-      <c r="D64" s="111"/>
-      <c r="E64" s="111"/>
-      <c r="F64" s="111"/>
-      <c r="G64" s="111"/>
-      <c r="H64" s="111"/>
-      <c r="I64" s="111"/>
-    </row>
-    <row r="65" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F65" s="111"/>
-      <c r="G65" s="111"/>
-      <c r="H65" s="111"/>
-      <c r="I65" s="111"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="G60" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11978,7 +10633,7 @@
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="72" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="119" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="116" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="76" customWidth="1"/>
     <col min="11" max="11" width="16.140625" style="74" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
@@ -11996,7 +10651,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -12005,7 +10660,7 @@
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
       <c r="H1" s="83"/>
-      <c r="I1" s="114"/>
+      <c r="I1" s="111"/>
       <c r="J1" s="84"/>
       <c r="K1" s="85"/>
       <c r="L1" s="49"/>
@@ -12021,8 +10676,8 @@
       <c r="V1" s="42"/>
     </row>
     <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="131" t="s">
-        <v>164</v>
+      <c r="A2" s="128" t="s">
+        <v>110</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -12031,7 +10686,7 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="83"/>
-      <c r="I2" s="114"/>
+      <c r="I2" s="111"/>
       <c r="J2" s="84"/>
       <c r="K2" s="85"/>
       <c r="L2" s="49"/>
@@ -12047,7 +10702,7 @@
       <c r="V2" s="42"/>
     </row>
     <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="131"/>
+      <c r="A3" s="128"/>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="60"/>
@@ -12055,14 +10710,14 @@
       <c r="F3" s="49"/>
       <c r="G3" s="49"/>
       <c r="H3" s="83"/>
-      <c r="I3" s="114"/>
+      <c r="I3" s="111"/>
       <c r="J3" s="84"/>
       <c r="K3" s="85"/>
       <c r="L3" s="49"/>
       <c r="M3" s="86"/>
       <c r="N3" s="49"/>
       <c r="O3" s="49"/>
-      <c r="P3" s="143" t="str">
+      <c r="P3" s="138" t="str">
         <f>Dashboard!O114</f>
         <v>Please see Key for Descriptions</v>
       </c>
@@ -12073,7 +10728,7 @@
       <c r="V3" s="42"/>
     </row>
     <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="137">
+      <c r="A4" s="132">
         <f>Dashboard!$J$4</f>
         <v>0</v>
       </c>
@@ -12084,7 +10739,7 @@
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
       <c r="H4" s="83"/>
-      <c r="I4" s="114"/>
+      <c r="I4" s="111"/>
       <c r="J4" s="84"/>
       <c r="K4" s="85"/>
       <c r="L4" s="49"/>
@@ -12108,7 +10763,7 @@
       <c r="F5" s="49"/>
       <c r="G5" s="49"/>
       <c r="H5" s="83"/>
-      <c r="I5" s="114"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="84"/>
       <c r="K5" s="85"/>
       <c r="L5" s="49"/>
@@ -12132,7 +10787,7 @@
       <c r="F6" s="49"/>
       <c r="G6" s="49"/>
       <c r="H6" s="83"/>
-      <c r="I6" s="114"/>
+      <c r="I6" s="111"/>
       <c r="J6" s="84"/>
       <c r="K6" s="85"/>
       <c r="L6" s="49"/>
@@ -12151,14 +10806,14 @@
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="69"/>
-      <c r="I7" s="115"/>
+      <c r="I7" s="112"/>
       <c r="J7" s="75" t="s">
         <v>64</v>
       </c>
@@ -12188,7 +10843,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="69"/>
-      <c r="I8" s="115"/>
+      <c r="I8" s="112"/>
       <c r="J8" s="75"/>
       <c r="K8" s="73"/>
       <c r="L8" s="11"/>
@@ -12211,7 +10866,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>57</v>
@@ -12226,10 +10881,10 @@
         <v>59</v>
       </c>
       <c r="H9" s="70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="70" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="J9" s="79" t="s">
         <v>56</v>
@@ -12275,7 +10930,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="17"/>
       <c r="H10" s="20"/>
-      <c r="I10" s="117"/>
+      <c r="I10" s="114"/>
       <c r="M10"/>
       <c r="N10" s="2"/>
       <c r="R10" s="19"/>
@@ -12286,7 +10941,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="17"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="117"/>
+      <c r="I11" s="114"/>
       <c r="M11"/>
       <c r="N11" s="2"/>
       <c r="R11" s="19"/>
@@ -12297,7 +10952,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="17"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="116"/>
+      <c r="I12" s="113"/>
       <c r="M12"/>
       <c r="N12" s="2"/>
       <c r="R12" s="19"/>
@@ -12309,7 +10964,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="17"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="117"/>
+      <c r="I13" s="114"/>
       <c r="M13"/>
       <c r="N13" s="2"/>
       <c r="R13" s="19"/>
@@ -12320,7 +10975,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="17"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="117"/>
+      <c r="I14" s="114"/>
       <c r="M14"/>
       <c r="N14" s="2"/>
       <c r="R14" s="19"/>
@@ -12330,7 +10985,7 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G15" s="28"/>
       <c r="H15" s="71"/>
-      <c r="I15" s="118"/>
+      <c r="I15" s="115"/>
       <c r="K15" s="68"/>
       <c r="O15" s="68"/>
       <c r="P15" s="66"/>
@@ -12344,7 +10999,7 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G16" s="28"/>
       <c r="H16" s="71"/>
-      <c r="I16" s="118"/>
+      <c r="I16" s="115"/>
       <c r="K16" s="68"/>
       <c r="O16" s="68"/>
       <c r="P16" s="66"/>
@@ -12358,7 +11013,7 @@
     <row r="17" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G17" s="28"/>
       <c r="H17" s="71"/>
-      <c r="I17" s="118"/>
+      <c r="I17" s="115"/>
       <c r="K17" s="68"/>
       <c r="P17" s="68"/>
       <c r="Q17" s="67"/>
@@ -12372,7 +11027,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="17"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="116"/>
+      <c r="I18" s="113"/>
       <c r="M18"/>
       <c r="N18" s="2"/>
       <c r="R18" s="19"/>
@@ -12383,7 +11038,7 @@
     <row r="19" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G19" s="28"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="118"/>
+      <c r="I19" s="115"/>
       <c r="K19" s="68"/>
       <c r="O19" s="68"/>
       <c r="P19" s="66"/>
@@ -12397,7 +11052,7 @@
     <row r="20" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G20" s="28"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="118"/>
+      <c r="I20" s="115"/>
       <c r="K20" s="68"/>
       <c r="O20" s="68"/>
       <c r="P20" s="66"/>
@@ -12411,7 +11066,7 @@
     <row r="21" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G21" s="28"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="118"/>
+      <c r="I21" s="115"/>
       <c r="K21" s="68"/>
       <c r="O21" s="68"/>
       <c r="P21" s="66"/>
@@ -12425,7 +11080,7 @@
     <row r="22" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G22" s="28"/>
       <c r="H22" s="71"/>
-      <c r="I22" s="118"/>
+      <c r="I22" s="115"/>
       <c r="K22" s="68"/>
       <c r="O22" s="68"/>
       <c r="P22" s="66"/>
@@ -12439,7 +11094,7 @@
     <row r="23" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G23" s="28"/>
       <c r="H23" s="71"/>
-      <c r="I23" s="118"/>
+      <c r="I23" s="115"/>
       <c r="K23" s="68"/>
       <c r="O23" s="68"/>
       <c r="P23" s="66"/>
@@ -12453,7 +11108,7 @@
     <row r="24" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G24" s="28"/>
       <c r="H24" s="71"/>
-      <c r="I24" s="118"/>
+      <c r="I24" s="115"/>
       <c r="K24" s="68"/>
       <c r="O24" s="68"/>
       <c r="P24" s="66"/>
@@ -12467,7 +11122,7 @@
     <row r="25" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G25" s="28"/>
       <c r="H25" s="71"/>
-      <c r="I25" s="118"/>
+      <c r="I25" s="115"/>
       <c r="K25" s="68"/>
       <c r="O25" s="68"/>
       <c r="P25" s="66"/>
@@ -12482,7 +11137,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="17"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="116"/>
+      <c r="I26" s="113"/>
       <c r="M26"/>
       <c r="N26" s="2"/>
       <c r="R26" s="19"/>
@@ -12494,7 +11149,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="17"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="116"/>
+      <c r="I27" s="113"/>
       <c r="M27"/>
       <c r="N27" s="2"/>
       <c r="R27" s="19"/>
@@ -12506,7 +11161,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="17"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="117"/>
+      <c r="I28" s="114"/>
       <c r="M28"/>
       <c r="N28" s="2"/>
       <c r="R28" s="19"/>
@@ -12518,7 +11173,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="17"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="117"/>
+      <c r="I29" s="114"/>
       <c r="M29"/>
       <c r="N29" s="2"/>
       <c r="R29" s="19"/>
@@ -12529,7 +11184,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="17"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="117"/>
+      <c r="I30" s="114"/>
       <c r="M30"/>
       <c r="N30" s="2"/>
       <c r="R30" s="19"/>
@@ -12540,7 +11195,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="17"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="117"/>
+      <c r="I31" s="114"/>
       <c r="M31"/>
       <c r="N31" s="2"/>
       <c r="R31" s="19"/>
@@ -12550,7 +11205,7 @@
     <row r="32" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G32" s="28"/>
       <c r="H32" s="71"/>
-      <c r="I32" s="118"/>
+      <c r="I32" s="115"/>
       <c r="K32" s="68"/>
       <c r="O32" s="68"/>
       <c r="P32" s="66"/>
@@ -12564,7 +11219,7 @@
     <row r="33" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G33" s="28"/>
       <c r="H33" s="71"/>
-      <c r="I33" s="118"/>
+      <c r="I33" s="115"/>
       <c r="K33" s="68"/>
       <c r="O33" s="68"/>
       <c r="P33" s="66"/>
@@ -12578,7 +11233,7 @@
     <row r="34" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G34" s="28"/>
       <c r="H34" s="71"/>
-      <c r="I34" s="118"/>
+      <c r="I34" s="115"/>
       <c r="K34" s="68"/>
       <c r="O34" s="68"/>
       <c r="P34" s="66"/>
@@ -12592,7 +11247,7 @@
     <row r="35" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G35" s="28"/>
       <c r="H35" s="71"/>
-      <c r="I35" s="118"/>
+      <c r="I35" s="115"/>
       <c r="K35" s="68"/>
       <c r="O35" s="68"/>
       <c r="P35" s="66"/>
@@ -12606,7 +11261,7 @@
     <row r="36" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G36" s="28"/>
       <c r="H36" s="71"/>
-      <c r="I36" s="118"/>
+      <c r="I36" s="115"/>
       <c r="K36" s="68"/>
       <c r="O36" s="68"/>
       <c r="P36" s="66"/>
@@ -12620,7 +11275,7 @@
     <row r="37" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G37" s="28"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="118"/>
+      <c r="I37" s="115"/>
       <c r="K37" s="68"/>
       <c r="O37" s="68"/>
       <c r="P37" s="66"/>
@@ -12634,7 +11289,7 @@
     <row r="38" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G38" s="28"/>
       <c r="H38" s="71"/>
-      <c r="I38" s="118"/>
+      <c r="I38" s="115"/>
       <c r="K38" s="68"/>
       <c r="O38" s="68"/>
       <c r="P38" s="66"/>
@@ -12648,7 +11303,7 @@
     <row r="39" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G39" s="28"/>
       <c r="H39" s="71"/>
-      <c r="I39" s="118"/>
+      <c r="I39" s="115"/>
       <c r="K39" s="68"/>
       <c r="O39" s="68"/>
       <c r="P39" s="66"/>
@@ -12662,7 +11317,7 @@
     <row r="40" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G40" s="28"/>
       <c r="H40" s="71"/>
-      <c r="I40" s="118"/>
+      <c r="I40" s="115"/>
       <c r="K40" s="68"/>
       <c r="O40" s="68"/>
       <c r="P40" s="66"/>
@@ -12676,7 +11331,7 @@
     <row r="41" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G41" s="28"/>
       <c r="H41" s="71"/>
-      <c r="I41" s="118"/>
+      <c r="I41" s="115"/>
       <c r="K41" s="68"/>
       <c r="O41" s="68"/>
       <c r="P41" s="66"/>
@@ -12690,7 +11345,7 @@
     <row r="42" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G42" s="28"/>
       <c r="H42" s="71"/>
-      <c r="I42" s="118"/>
+      <c r="I42" s="115"/>
       <c r="K42" s="68"/>
       <c r="O42" s="68"/>
       <c r="P42" s="66"/>
@@ -12704,7 +11359,7 @@
     <row r="43" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G43" s="28"/>
       <c r="H43" s="71"/>
-      <c r="I43" s="118"/>
+      <c r="I43" s="115"/>
       <c r="K43" s="68"/>
       <c r="P43" s="68"/>
       <c r="Q43" s="67"/>
@@ -12717,7 +11372,7 @@
     <row r="44" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G44" s="28"/>
       <c r="H44" s="71"/>
-      <c r="I44" s="118"/>
+      <c r="I44" s="115"/>
       <c r="K44" s="68"/>
       <c r="P44" s="68"/>
       <c r="Q44" s="67"/>
@@ -12730,7 +11385,7 @@
     <row r="45" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G45" s="28"/>
       <c r="H45" s="71"/>
-      <c r="I45" s="118"/>
+      <c r="I45" s="115"/>
       <c r="K45" s="68"/>
       <c r="O45" s="68"/>
       <c r="P45" s="66"/>
@@ -12744,7 +11399,7 @@
     <row r="46" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G46" s="28"/>
       <c r="H46" s="71"/>
-      <c r="I46" s="118"/>
+      <c r="I46" s="115"/>
       <c r="K46" s="68"/>
       <c r="O46" s="68"/>
       <c r="P46" s="66"/>
@@ -12758,7 +11413,7 @@
     <row r="47" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G47" s="28"/>
       <c r="H47" s="71"/>
-      <c r="I47" s="118"/>
+      <c r="I47" s="115"/>
       <c r="K47" s="68"/>
       <c r="O47" s="68"/>
       <c r="P47" s="66"/>
@@ -12773,7 +11428,7 @@
       <c r="F48" s="8"/>
       <c r="G48" s="17"/>
       <c r="H48" s="20"/>
-      <c r="I48" s="116"/>
+      <c r="I48" s="113"/>
       <c r="M48"/>
       <c r="N48" s="2"/>
       <c r="R48" s="19"/>
@@ -12784,7 +11439,7 @@
     <row r="49" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G49" s="28"/>
       <c r="H49" s="71"/>
-      <c r="I49" s="118"/>
+      <c r="I49" s="115"/>
       <c r="K49" s="68"/>
       <c r="O49" s="68"/>
       <c r="P49" s="66"/>
@@ -12798,7 +11453,7 @@
     <row r="50" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G50" s="28"/>
       <c r="H50" s="71"/>
-      <c r="I50" s="118"/>
+      <c r="I50" s="115"/>
       <c r="K50" s="68"/>
       <c r="O50" s="68"/>
       <c r="P50" s="66"/>
@@ -12812,7 +11467,7 @@
     <row r="51" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G51" s="28"/>
       <c r="H51" s="71"/>
-      <c r="I51" s="118"/>
+      <c r="I51" s="115"/>
       <c r="K51" s="68"/>
       <c r="O51" s="68"/>
       <c r="P51" s="66"/>
@@ -12826,7 +11481,7 @@
     <row r="52" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G52" s="28"/>
       <c r="H52" s="71"/>
-      <c r="I52" s="118"/>
+      <c r="I52" s="115"/>
       <c r="K52" s="68"/>
       <c r="O52" s="68"/>
       <c r="P52" s="66"/>
@@ -12840,7 +11495,7 @@
     <row r="53" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G53" s="28"/>
       <c r="H53" s="71"/>
-      <c r="I53" s="118"/>
+      <c r="I53" s="115"/>
       <c r="K53" s="68"/>
       <c r="O53" s="68"/>
       <c r="P53" s="66"/>
@@ -12854,7 +11509,7 @@
     <row r="54" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
       <c r="H54" s="71"/>
-      <c r="I54" s="118"/>
+      <c r="I54" s="115"/>
       <c r="K54" s="68"/>
       <c r="O54" s="68"/>
       <c r="P54" s="66"/>
@@ -12868,7 +11523,7 @@
     <row r="55" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G55" s="28"/>
       <c r="H55" s="71"/>
-      <c r="I55" s="118"/>
+      <c r="I55" s="115"/>
       <c r="K55" s="68"/>
       <c r="O55" s="68"/>
       <c r="P55" s="66"/>
@@ -12882,7 +11537,7 @@
     <row r="56" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G56" s="28"/>
       <c r="H56" s="71"/>
-      <c r="I56" s="118"/>
+      <c r="I56" s="115"/>
       <c r="K56" s="68"/>
       <c r="O56" s="68"/>
       <c r="P56" s="66"/>
@@ -12896,7 +11551,7 @@
     <row r="57" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G57" s="28"/>
       <c r="H57" s="71"/>
-      <c r="I57" s="118"/>
+      <c r="I57" s="115"/>
       <c r="K57" s="68"/>
       <c r="O57" s="68"/>
       <c r="P57" s="66"/>
@@ -12910,7 +11565,7 @@
     <row r="58" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G58" s="28"/>
       <c r="H58" s="71"/>
-      <c r="I58" s="118"/>
+      <c r="I58" s="115"/>
       <c r="K58" s="68"/>
       <c r="O58" s="68"/>
       <c r="P58" s="66"/>
@@ -12924,7 +11579,7 @@
     <row r="59" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G59" s="28"/>
       <c r="H59" s="71"/>
-      <c r="I59" s="118"/>
+      <c r="I59" s="115"/>
       <c r="K59" s="68"/>
       <c r="O59" s="68"/>
       <c r="P59" s="66"/>
@@ -12938,7 +11593,7 @@
     <row r="60" spans="6:22" x14ac:dyDescent="0.2">
       <c r="G60" s="28"/>
       <c r="H60" s="71"/>
-      <c r="I60" s="118"/>
+      <c r="I60" s="115"/>
       <c r="K60" s="68"/>
       <c r="O60" s="68"/>
       <c r="P60" s="66"/>
@@ -12953,7 +11608,7 @@
       <c r="F61" s="8"/>
       <c r="G61" s="17"/>
       <c r="H61" s="20"/>
-      <c r="I61" s="116"/>
+      <c r="I61" s="113"/>
       <c r="M61"/>
       <c r="N61" s="2"/>
       <c r="R61" s="19"/>
@@ -12962,7 +11617,7 @@
       <c r="F62" s="8"/>
       <c r="G62" s="17"/>
       <c r="H62" s="20"/>
-      <c r="I62" s="116"/>
+      <c r="I62" s="113"/>
       <c r="M62"/>
       <c r="N62" s="2"/>
       <c r="R62" s="19"/>
@@ -12971,7 +11626,7 @@
       <c r="F63" s="8"/>
       <c r="G63" s="17"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="116"/>
+      <c r="I63" s="113"/>
       <c r="M63"/>
       <c r="N63" s="2"/>
       <c r="R63" s="19"/>
@@ -12980,7 +11635,7 @@
       <c r="F64" s="8"/>
       <c r="G64" s="17"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="116"/>
+      <c r="I64" s="113"/>
       <c r="M64"/>
       <c r="N64" s="2"/>
       <c r="R64" s="19"/>
@@ -12989,7 +11644,7 @@
       <c r="F65" s="8"/>
       <c r="G65" s="17"/>
       <c r="H65" s="20"/>
-      <c r="I65" s="117"/>
+      <c r="I65" s="114"/>
       <c r="M65"/>
       <c r="N65" s="2"/>
       <c r="R65" s="19"/>
@@ -13001,7 +11656,7 @@
       <c r="F66" s="8"/>
       <c r="G66" s="17"/>
       <c r="H66" s="20"/>
-      <c r="I66" s="117"/>
+      <c r="I66" s="114"/>
       <c r="M66"/>
       <c r="N66" s="2"/>
       <c r="R66" s="19"/>
@@ -13013,7 +11668,7 @@
       <c r="F67" s="8"/>
       <c r="G67" s="17"/>
       <c r="H67" s="20"/>
-      <c r="I67" s="117"/>
+      <c r="I67" s="114"/>
       <c r="M67"/>
       <c r="N67" s="2"/>
       <c r="R67" s="19"/>
@@ -13025,7 +11680,7 @@
       <c r="F68" s="8"/>
       <c r="G68" s="17"/>
       <c r="H68" s="20"/>
-      <c r="I68" s="117"/>
+      <c r="I68" s="114"/>
       <c r="M68"/>
       <c r="N68" s="2"/>
       <c r="O68" s="68"/>
@@ -13037,7 +11692,7 @@
       <c r="F69" s="8"/>
       <c r="G69" s="17"/>
       <c r="H69" s="20"/>
-      <c r="I69" s="117"/>
+      <c r="I69" s="114"/>
       <c r="M69"/>
       <c r="N69" s="2"/>
       <c r="R69" s="19"/>
@@ -13048,7 +11703,7 @@
       <c r="F70" s="8"/>
       <c r="G70" s="17"/>
       <c r="H70" s="20"/>
-      <c r="I70" s="117"/>
+      <c r="I70" s="114"/>
       <c r="M70"/>
       <c r="N70" s="2"/>
       <c r="R70" s="19"/>
@@ -13059,7 +11714,7 @@
       <c r="F71" s="8"/>
       <c r="G71" s="17"/>
       <c r="H71" s="20"/>
-      <c r="I71" s="117"/>
+      <c r="I71" s="114"/>
       <c r="M71"/>
       <c r="N71" s="2"/>
       <c r="R71" s="19"/>
@@ -13070,7 +11725,7 @@
       <c r="F72" s="8"/>
       <c r="G72" s="17"/>
       <c r="H72" s="20"/>
-      <c r="I72" s="117"/>
+      <c r="I72" s="114"/>
       <c r="M72"/>
       <c r="N72" s="2"/>
       <c r="R72" s="19"/>
@@ -13081,7 +11736,7 @@
       <c r="F73" s="8"/>
       <c r="G73" s="17"/>
       <c r="H73" s="20"/>
-      <c r="I73" s="117"/>
+      <c r="I73" s="114"/>
       <c r="M73"/>
       <c r="N73" s="2"/>
       <c r="R73" s="19"/>
@@ -13092,7 +11747,7 @@
       <c r="F74" s="8"/>
       <c r="G74" s="17"/>
       <c r="H74" s="20"/>
-      <c r="I74" s="117"/>
+      <c r="I74" s="114"/>
       <c r="M74"/>
       <c r="N74" s="2"/>
       <c r="R74" s="19"/>
@@ -13103,7 +11758,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="17"/>
       <c r="H75" s="20"/>
-      <c r="I75" s="117"/>
+      <c r="I75" s="114"/>
       <c r="M75"/>
       <c r="N75" s="2"/>
       <c r="R75" s="19"/>
@@ -13114,7 +11769,7 @@
       <c r="F76" s="8"/>
       <c r="G76" s="17"/>
       <c r="H76" s="20"/>
-      <c r="I76" s="117"/>
+      <c r="I76" s="114"/>
       <c r="M76"/>
       <c r="N76" s="2"/>
       <c r="O76" s="68"/>
@@ -13126,7 +11781,7 @@
       <c r="F77" s="8"/>
       <c r="G77" s="17"/>
       <c r="H77" s="20"/>
-      <c r="I77" s="117"/>
+      <c r="I77" s="114"/>
       <c r="M77"/>
       <c r="N77" s="2"/>
       <c r="R77" s="19"/>
@@ -13137,7 +11792,7 @@
       <c r="F78" s="8"/>
       <c r="G78" s="17"/>
       <c r="H78" s="20"/>
-      <c r="I78" s="117"/>
+      <c r="I78" s="114"/>
       <c r="M78"/>
       <c r="N78" s="2"/>
       <c r="R78" s="19"/>
@@ -13148,7 +11803,7 @@
       <c r="F79" s="8"/>
       <c r="G79" s="17"/>
       <c r="H79" s="20"/>
-      <c r="I79" s="117"/>
+      <c r="I79" s="114"/>
       <c r="M79"/>
       <c r="N79" s="2"/>
       <c r="R79" s="19"/>
@@ -13159,7 +11814,7 @@
       <c r="F80" s="8"/>
       <c r="G80" s="17"/>
       <c r="H80" s="20"/>
-      <c r="I80" s="117"/>
+      <c r="I80" s="114"/>
       <c r="M80"/>
       <c r="N80" s="2"/>
       <c r="R80" s="19"/>
@@ -13170,7 +11825,7 @@
       <c r="F81" s="8"/>
       <c r="G81" s="17"/>
       <c r="H81" s="20"/>
-      <c r="I81" s="117"/>
+      <c r="I81" s="114"/>
       <c r="M81"/>
       <c r="N81" s="2"/>
       <c r="R81" s="19"/>
@@ -13181,7 +11836,7 @@
       <c r="F82" s="8"/>
       <c r="G82" s="17"/>
       <c r="H82" s="20"/>
-      <c r="I82" s="117"/>
+      <c r="I82" s="114"/>
       <c r="M82"/>
       <c r="N82" s="2"/>
       <c r="R82" s="19"/>
@@ -13192,7 +11847,7 @@
       <c r="F83" s="8"/>
       <c r="G83" s="17"/>
       <c r="H83" s="20"/>
-      <c r="I83" s="117"/>
+      <c r="I83" s="114"/>
       <c r="M83"/>
       <c r="N83" s="2"/>
       <c r="R83" s="19"/>
@@ -13203,7 +11858,7 @@
       <c r="F84" s="8"/>
       <c r="G84" s="17"/>
       <c r="H84" s="20"/>
-      <c r="I84" s="117"/>
+      <c r="I84" s="114"/>
       <c r="M84"/>
       <c r="N84" s="2"/>
       <c r="O84" s="68"/>
@@ -13215,7 +11870,7 @@
       <c r="F85" s="8"/>
       <c r="G85" s="17"/>
       <c r="H85" s="20"/>
-      <c r="I85" s="117"/>
+      <c r="I85" s="114"/>
       <c r="M85"/>
       <c r="N85" s="2"/>
       <c r="O85" s="68"/>
@@ -13227,7 +11882,7 @@
       <c r="F86" s="8"/>
       <c r="G86" s="17"/>
       <c r="H86" s="20"/>
-      <c r="I86" s="117"/>
+      <c r="I86" s="114"/>
       <c r="M86"/>
       <c r="N86" s="2"/>
       <c r="O86" s="68"/>
@@ -13239,7 +11894,7 @@
       <c r="F87" s="8"/>
       <c r="G87" s="17"/>
       <c r="H87" s="20"/>
-      <c r="I87" s="117"/>
+      <c r="I87" s="114"/>
       <c r="M87"/>
       <c r="N87" s="2"/>
       <c r="O87" s="68"/>
@@ -13251,7 +11906,7 @@
       <c r="F88" s="8"/>
       <c r="G88" s="17"/>
       <c r="H88" s="20"/>
-      <c r="I88" s="117"/>
+      <c r="I88" s="114"/>
       <c r="M88"/>
       <c r="N88" s="2"/>
       <c r="O88" s="68"/>
@@ -13263,7 +11918,7 @@
       <c r="F89" s="8"/>
       <c r="G89" s="17"/>
       <c r="H89" s="20"/>
-      <c r="I89" s="117"/>
+      <c r="I89" s="114"/>
       <c r="M89"/>
       <c r="N89" s="2"/>
       <c r="R89" s="19"/>
@@ -13274,7 +11929,7 @@
       <c r="F90" s="8"/>
       <c r="G90" s="17"/>
       <c r="H90" s="20"/>
-      <c r="I90" s="117"/>
+      <c r="I90" s="114"/>
       <c r="M90"/>
       <c r="N90" s="2"/>
       <c r="O90" s="68"/>
@@ -13286,7 +11941,7 @@
       <c r="F91" s="8"/>
       <c r="G91" s="17"/>
       <c r="H91" s="20"/>
-      <c r="I91" s="117"/>
+      <c r="I91" s="114"/>
       <c r="M91"/>
       <c r="N91" s="2"/>
       <c r="O91" s="68"/>
@@ -13298,7 +11953,7 @@
       <c r="F92" s="8"/>
       <c r="G92" s="17"/>
       <c r="H92" s="20"/>
-      <c r="I92" s="117"/>
+      <c r="I92" s="114"/>
       <c r="M92"/>
       <c r="N92" s="2"/>
       <c r="O92" s="68"/>
@@ -13310,7 +11965,7 @@
       <c r="F93" s="8"/>
       <c r="G93" s="17"/>
       <c r="H93" s="20"/>
-      <c r="I93" s="117"/>
+      <c r="I93" s="114"/>
       <c r="M93"/>
       <c r="N93" s="2"/>
       <c r="O93" s="68"/>
@@ -16057,7 +14712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16078,10 +14733,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="167" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="167"/>
+      <c r="A1" s="161" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="161"/>
       <c r="C1" s="45"/>
       <c r="D1" s="42"/>
     </row>
@@ -16098,27 +14753,27 @@
       <c r="D3" s="42"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="145" t="s">
-        <v>178</v>
-      </c>
-      <c r="B4" s="140" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" s="140" t="s">
+      <c r="A4" s="140" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="135" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="136" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="90" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="124" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="121" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="92"/>
@@ -16128,13 +14783,13 @@
         <v>33</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="124" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="121" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
@@ -16145,9 +14800,9 @@
         <v>34</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="124">
+        <v>106</v>
+      </c>
+      <c r="C7" s="121">
         <v>1</v>
       </c>
       <c r="D7" s="96"/>
@@ -16157,12 +14812,12 @@
     </row>
     <row r="8" spans="1:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="124">
+        <v>100</v>
+      </c>
+      <c r="C8" s="121">
         <v>5</v>
       </c>
       <c r="D8" s="96"/>
@@ -16172,12 +14827,12 @@
     </row>
     <row r="9" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="124">
+        <v>102</v>
+      </c>
+      <c r="C9" s="121">
         <v>10</v>
       </c>
       <c r="D9" s="96"/>
@@ -16190,9 +14845,9 @@
         <v>35</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="124">
+        <v>105</v>
+      </c>
+      <c r="C10" s="121">
         <v>15</v>
       </c>
       <c r="D10" s="96"/>
@@ -16205,13 +14860,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="125" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="122" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="99" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -16220,7 +14875,7 @@
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="100"/>
       <c r="B12" s="101"/>
-      <c r="C12" s="126"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="102"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -16229,7 +14884,7 @@
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="100"/>
       <c r="B13" s="101"/>
-      <c r="C13" s="126"/>
+      <c r="C13" s="123"/>
       <c r="D13" s="102"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -16238,7 +14893,7 @@
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="100"/>
       <c r="B14" s="101"/>
-      <c r="C14" s="126"/>
+      <c r="C14" s="123"/>
       <c r="D14" s="102"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -16247,13 +14902,13 @@
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="100"/>
       <c r="B15" s="101"/>
-      <c r="C15" s="126"/>
+      <c r="C15" s="123"/>
       <c r="D15" s="102"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="100"/>
       <c r="B16" s="101"/>
-      <c r="C16" s="126"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="102"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
TICKET2383 - Consolidated Report * Updated Excel template. I won't pretend to remember what the exact change was.
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3620 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-2.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4605" windowWidth="19440" windowHeight="10800" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="4605" windowWidth="19440" windowHeight="10800" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Activity Summary'!$A$1:$I$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Bookings!$A$1:$I$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Contact Details'!$A$1:$S$93</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Impressions!$A$1:$P$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Impressions!$A$1:$P$28</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'Contact Details'!$9:$9</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
   <si>
     <t>calls</t>
   </si>
@@ -1598,16 +1598,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3401.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4150</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8950</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1855,10 +1855,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>495</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>335</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1952,10 +1952,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>625</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>270</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2049,10 +2049,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>495</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2382,6 +2382,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2779,15 +2780,6 @@
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2956,6 +2948,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3022,7 +3015,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Impressions!$N$18</c:f>
+              <c:f>Impressions!$N$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3047,7 +3040,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Impressions!$A$19:$A$25</c:f>
+              <c:f>Impressions!$A$18:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -3076,7 +3069,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Impressions!$N$19:$N$25</c:f>
+              <c:f>Impressions!$N$18:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3362,7 +3355,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4535</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3832,8 +3825,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -3905,8 +3898,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -7218,8 +7211,8 @@
   </sheetPr>
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7227,7 +7220,7 @@
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="11" max="13" width="11.42578125" customWidth="1"/>
@@ -7403,14 +7396,8 @@
         <f>E26/5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F11" s="8">
-        <f>Impressions!F10</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="158" t="e">
-        <f>G26/5</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="158"/>
       <c r="H11" s="8">
         <f t="shared" ref="H11:I13" si="0">B11+D11+F11</f>
         <v>0</v>
@@ -7427,36 +7414,28 @@
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="8">
-        <f>0.03*B11</f>
-        <v>0</v>
-      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="17">
         <f>B12*$J12</f>
         <v>0</v>
       </c>
-      <c r="D12" s="8">
-        <v>907</v>
-      </c>
+      <c r="D12" s="8"/>
       <c r="E12" s="17">
         <f>D12*$J12</f>
-        <v>680.25</v>
-      </c>
-      <c r="F12" s="8">
-        <f>0*F11</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="17">
         <f>F12*$J12</f>
         <v>0</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="0"/>
-        <v>907</v>
+        <v>0</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" si="0"/>
-        <v>680.25</v>
+        <v>0</v>
       </c>
       <c r="J12" s="18">
         <v>0.75</v>
@@ -7466,34 +7445,28 @@
       <c r="A13" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="8">
-        <v>99</v>
-      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="17">
         <f>B13*$J13</f>
-        <v>495</v>
-      </c>
-      <c r="D13" s="8">
-        <v>67</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="17">
         <f>D13*$J13</f>
-        <v>335</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="17">
         <f>F13*$J13</f>
         <v>0</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" si="0"/>
-        <v>830</v>
+        <v>0</v>
       </c>
       <c r="J13" s="18">
         <f>'Key - Legend'!C8</f>
@@ -7504,34 +7477,28 @@
       <c r="A14" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="8">
-        <v>125</v>
-      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="17">
         <f t="shared" ref="C14:E15" si="1">B14*$J14</f>
-        <v>1250</v>
-      </c>
-      <c r="D14" s="8">
-        <v>54</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="17">
         <f t="shared" si="1"/>
-        <v>540</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="17">
         <f>F14*$J14</f>
         <v>0</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" ref="H14:I18" si="2">B14+D14+F14</f>
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="I14" s="17">
         <f>C14+E14+G14</f>
-        <v>1790</v>
+        <v>0</v>
       </c>
       <c r="J14" s="18">
         <f>'Key - Legend'!C9</f>
@@ -7542,34 +7509,28 @@
       <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="8">
-        <v>99</v>
-      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="17">
         <f t="shared" si="1"/>
-        <v>1485</v>
-      </c>
-      <c r="D15" s="8">
-        <v>41</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="17">
         <f t="shared" si="1"/>
-        <v>615</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="17">
         <f>F15*$J15</f>
         <v>0</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="2"/>
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="I15" s="17">
         <f t="shared" si="2"/>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="J15" s="18">
         <f>'Key - Legend'!C10</f>
@@ -7591,9 +7552,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="23" t="e">
+      <c r="G16" s="23">
         <f>SUM(G11:G15)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="23" t="e">
@@ -7667,9 +7628,9 @@
         <f>E16+E18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="28" t="e">
+      <c r="G19" s="28">
         <f>G16+G18</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="I19" s="39" t="e">
         <f>I16+I18</f>
@@ -7780,14 +7741,8 @@
         <f>Impressions!O9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F26" s="8">
-        <f>Impressions!N10</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="17" t="e">
-        <f>Impressions!O10</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="8">
         <f t="shared" ref="H26:I30" si="3">B26+D26+F26</f>
         <v>0</v>
@@ -7805,36 +7760,28 @@
       <c r="A27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="8">
-        <f>B12*5</f>
-        <v>0</v>
-      </c>
+      <c r="B27" s="8"/>
       <c r="C27" s="17">
         <f>B27*$J27</f>
         <v>0</v>
       </c>
-      <c r="D27" s="8">
-        <f>D12*5</f>
-        <v>4535</v>
-      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="17">
         <f>D27*$J27</f>
-        <v>3401.25</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F27" s="8"/>
       <c r="G27" s="17">
         <f>F27*$J27</f>
         <v>0</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="3"/>
-        <v>4535</v>
+        <v>0</v>
       </c>
       <c r="I27" s="17">
         <f t="shared" si="3"/>
-        <v>3401.25</v>
+        <v>0</v>
       </c>
       <c r="J27" s="18">
         <f>J12</f>
@@ -7845,37 +7792,28 @@
       <c r="A28" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="8">
-        <f>B13*5</f>
-        <v>495</v>
-      </c>
+      <c r="B28" s="8"/>
       <c r="C28" s="17">
         <f>B28*$J28</f>
-        <v>2475</v>
-      </c>
-      <c r="D28" s="8">
-        <f>D13*5</f>
-        <v>335</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D28" s="8"/>
       <c r="E28" s="17">
         <f>D28*$J28</f>
-        <v>1675</v>
-      </c>
-      <c r="F28" s="8">
-        <f>F13*5</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="17">
         <f>F28*$J28</f>
         <v>0</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="3"/>
-        <v>830</v>
+        <v>0</v>
       </c>
       <c r="I28" s="17">
         <f t="shared" si="3"/>
-        <v>4150</v>
+        <v>0</v>
       </c>
       <c r="J28" s="18">
         <f>J13</f>
@@ -7886,37 +7824,28 @@
       <c r="A29" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="8">
-        <f>B14*5</f>
-        <v>625</v>
-      </c>
+      <c r="B29" s="8"/>
       <c r="C29" s="17">
         <f>B29*$J29</f>
-        <v>6250</v>
-      </c>
-      <c r="D29" s="8">
-        <f>D14*5</f>
-        <v>270</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="17">
         <f>D29*$J29</f>
-        <v>2700</v>
-      </c>
-      <c r="F29" s="8">
-        <f>F14*5</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F29" s="8"/>
       <c r="G29" s="17">
         <f>F29*$J29</f>
         <v>0</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="3"/>
-        <v>895</v>
+        <v>0</v>
       </c>
       <c r="I29" s="17">
         <f t="shared" si="3"/>
-        <v>8950</v>
+        <v>0</v>
       </c>
       <c r="J29" s="18">
         <f>J14</f>
@@ -7927,37 +7856,28 @@
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="8">
-        <f>B15*5</f>
-        <v>495</v>
-      </c>
+      <c r="B30" s="8"/>
       <c r="C30" s="17">
         <f>B30*$J30</f>
-        <v>7425</v>
-      </c>
-      <c r="D30" s="8">
-        <f>D15*5</f>
-        <v>205</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="17">
         <f>D30*$J30</f>
-        <v>3075</v>
-      </c>
-      <c r="F30" s="8">
-        <f>F15*5</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="17">
         <f>F30*$J30</f>
         <v>0</v>
       </c>
       <c r="H30" s="8">
         <f t="shared" si="3"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="I30" s="17">
         <f t="shared" si="3"/>
-        <v>10500</v>
+        <v>0</v>
       </c>
       <c r="J30" s="18">
         <f>J15</f>
@@ -7982,9 +7902,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="23" t="e">
+      <c r="G31" s="23">
         <f>SUM(G26:G30)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="23" t="e">
@@ -8065,9 +7985,9 @@
         <f>E31+E33</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G34" s="28" t="e">
+      <c r="G34" s="28">
         <f>G31+G33</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="I34" s="39" t="e">
         <f>I31+I33</f>
@@ -8516,7 +8436,7 @@
       </c>
       <c r="C73" s="9">
         <f t="shared" si="4"/>
-        <v>4535</v>
+        <v>0</v>
       </c>
       <c r="D73" s="9">
         <f t="shared" si="5"/>
@@ -8530,11 +8450,11 @@
       </c>
       <c r="B74" s="9">
         <f t="shared" si="6"/>
-        <v>495</v>
+        <v>0</v>
       </c>
       <c r="C74" s="9">
         <f t="shared" si="4"/>
-        <v>335</v>
+        <v>0</v>
       </c>
       <c r="D74" s="9">
         <f t="shared" si="5"/>
@@ -8548,11 +8468,11 @@
       </c>
       <c r="B75" s="9">
         <f t="shared" si="6"/>
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="C75" s="9">
         <f t="shared" si="4"/>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="D75" s="9">
         <f t="shared" si="5"/>
@@ -8566,11 +8486,11 @@
       </c>
       <c r="B76" s="9">
         <f t="shared" si="6"/>
-        <v>495</v>
+        <v>0</v>
       </c>
       <c r="C76" s="9">
         <f t="shared" si="4"/>
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D76" s="9">
         <f t="shared" si="5"/>
@@ -8616,8 +8536,8 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:G29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8627,8 +8547,8 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="0.85546875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="255" width="11.42578125" customWidth="1"/>
@@ -8727,10 +8647,7 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="17">
-        <f>D7*260</f>
-        <v>0</v>
-      </c>
+      <c r="E7" s="17"/>
       <c r="F7" s="29">
         <v>0.21</v>
       </c>
@@ -8746,10 +8663,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="17">
-        <f>D8*260</f>
-        <v>0</v>
-      </c>
+      <c r="E8" s="17"/>
       <c r="F8" s="29">
         <v>0.21</v>
       </c>
@@ -8765,10 +8679,7 @@
       <c r="B9" s="159"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="17">
-        <f>D9*260</f>
-        <v>0</v>
-      </c>
+      <c r="E9" s="17"/>
       <c r="F9" s="29">
         <v>0.18</v>
       </c>
@@ -8799,10 +8710,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E11" s="23"/>
       <c r="F11" s="29"/>
       <c r="G11" s="23">
         <f t="shared" si="0"/>
@@ -8888,10 +8796,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="17">
-        <f>D18*260</f>
-        <v>0</v>
-      </c>
+      <c r="E18" s="17"/>
       <c r="F18" s="29">
         <v>0.21</v>
       </c>
@@ -8907,10 +8812,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="17">
-        <f>D19*260</f>
-        <v>0</v>
-      </c>
+      <c r="E19" s="17"/>
       <c r="F19" s="29">
         <v>0.21</v>
       </c>
@@ -8926,10 +8828,7 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="17">
-        <f>D20*260</f>
-        <v>0</v>
-      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="29">
         <v>0.18</v>
       </c>
@@ -8960,10 +8859,7 @@
         <f>SUM(D18:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="23">
-        <f>SUM(E18:E21)</f>
-        <v>0</v>
-      </c>
+      <c r="E22" s="23"/>
       <c r="F22" s="29"/>
       <c r="G22" s="23">
         <f>SUM(G18:G21)</f>
@@ -9247,10 +9143,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9258,8 +9154,8 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7" hidden="1" customWidth="1"/>
     <col min="17" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9423,7 +9319,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="28" t="e">
-        <f>N8/N$12*O$27</f>
+        <f>N8/N$11*O$26</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P8" s="42"/>
@@ -9449,15 +9345,12 @@
         <v>0</v>
       </c>
       <c r="O9" s="28" t="e">
-        <f>N9/N$12*O$27</f>
+        <f>N9/N$11*O$26</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="42"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
+    <row r="10" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -9470,92 +9363,87 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="62">
-        <f>SUM(B10:M10)</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="28" t="e">
-        <f>N10/N$12*O$27</f>
+      <c r="N10" s="62"/>
+      <c r="P10" s="42"/>
+    </row>
+    <row r="11" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="25">
+        <f>SUM(B8:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="25">
+        <f>SUM(C8:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="25">
+        <f>SUM(D8:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="25">
+        <f>SUM(E8:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="25">
+        <f>SUM(F8:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="25">
+        <f>SUM(G8:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="25">
+        <f>SUM(H8:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="25">
+        <f>SUM(I8:I9)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="25">
+        <f>SUM(J8:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="25">
+        <f>SUM(K8:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="25">
+        <f>SUM(L8:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="25">
+        <f>SUM(M8:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="63">
+        <f>SUM(B11:M11)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="41" t="e">
+        <f>SUM(O8:O9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="42"/>
-    </row>
-    <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="62"/>
       <c r="P11" s="42"/>
     </row>
-    <row r="12" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="25">
-        <f t="shared" ref="B12:M12" si="0">SUM(B8:B10)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="63">
-        <f>SUM(B12:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="41" t="e">
-        <f>SUM(O8:O10)</f>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
       <c r="P12" s="42"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -9630,89 +9518,99 @@
       <c r="O16" s="42"/>
       <c r="P16" s="42"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="33">
-        <f t="shared" ref="B18:M18" si="1">B7</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="117" t="s">
+      <c r="B17" s="33">
+        <f>B7</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="33">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <f>F7</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <f>G7</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="33">
+        <f>H7</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <f>J7</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="33">
+        <f>K7</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="33">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="33">
+        <f>M7</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="O18" s="118" t="s">
+      <c r="O17" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="P18" s="40" t="s">
+      <c r="P17" s="40" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="62">
+        <f t="shared" ref="N18:N24" si="0">SUM(B18:M18)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="28">
+        <f>(N18/1000)*P18</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="17">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -9727,20 +9625,20 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="62">
-        <f t="shared" ref="N19:N25" si="2">SUM(B19:M19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O19" s="28">
-        <f>(N19/1000)*P19</f>
+        <f t="shared" ref="O19:O24" si="1">(N19/1000)*P19</f>
         <v>0</v>
       </c>
       <c r="P19" s="17">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -9755,20 +9653,20 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O20" s="28">
-        <f t="shared" ref="O20:O25" si="3">(N20/1000)*P20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="17">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -9783,20 +9681,20 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O21" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="17">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -9811,20 +9709,20 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O22" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -9839,20 +9737,20 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O23" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="17">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -9867,21 +9765,19 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O24" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P24" s="17">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>77</v>
-      </c>
+    <row r="25" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -9894,98 +9790,90 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="62">
+      <c r="N25" s="62"/>
+    </row>
+    <row r="26" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="26">
+        <f>SUM(B18:B24)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="26">
+        <f t="shared" ref="C26:M26" si="2">SUM(C18:C24)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="62"/>
-    </row>
-    <row r="27" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="26">
-        <f>SUM(B19:B25)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="26">
-        <f t="shared" ref="C27:M27" si="4">SUM(C19:C25)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="63">
-        <f>SUM(B27:M27)</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="41">
-        <f>SUM(O19:O25)</f>
-        <v>0</v>
-      </c>
+      <c r="E26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="63">
+        <f>SUM(B26:M26)</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="41">
+        <f>SUM(O18:O24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
@@ -10003,7 +9891,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
-      <c r="B29" s="65"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>
       <c r="E29" s="42"/>
@@ -10087,7 +9975,10 @@
       <c r="K33" s="42"/>
       <c r="L33" s="42"/>
       <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
+      <c r="N33" s="138" t="str">
+        <f>Dashboard!$O$114</f>
+        <v>Please see Key for Descriptions</v>
+      </c>
       <c r="O33" s="42"/>
       <c r="P33" s="42"/>
     </row>
@@ -10105,10 +9996,7 @@
       <c r="K34" s="42"/>
       <c r="L34" s="42"/>
       <c r="M34" s="42"/>
-      <c r="N34" s="138" t="str">
-        <f>Dashboard!$O$114</f>
-        <v>Please see Key for Descriptions</v>
-      </c>
+      <c r="N34" s="42"/>
       <c r="O34" s="42"/>
       <c r="P34" s="42"/>
     </row>
@@ -10134,7 +10022,7 @@
       <c r="A36" s="42"/>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
@@ -10188,7 +10076,7 @@
       <c r="A39" s="42"/>
       <c r="B39" s="42"/>
       <c r="C39" s="42"/>
-      <c r="D39" s="64"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
@@ -10580,28 +10468,10 @@
       <c r="O60" s="42"/>
       <c r="P60" s="42"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="42"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="42"/>
-      <c r="J61" s="42"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="42"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="42"/>
-      <c r="O61" s="42"/>
-      <c r="P61" s="42"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N34" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
+    <hyperlink ref="N33" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>